<commit_message>
I am an idiot
</commit_message>
<xml_diff>
--- a/inst/extdata/CAMERA_rules_neg.xlsx
+++ b/inst/extdata/CAMERA_rules_neg.xlsx
@@ -944,8 +944,8 @@
   <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4163,8 +4163,8 @@
         <v>-1</v>
       </c>
       <c r="D139">
-        <f>-(162.05283+D2)</f>
-        <v>-161.04555354499999</v>
+        <f>-(162.05283-D2)</f>
+        <v>-163.06010645500001</v>
       </c>
       <c r="E139" s="15">
         <v>173</v>

</xml_diff>

<commit_message>
added more friends to glucose fragments
</commit_message>
<xml_diff>
--- a/inst/extdata/CAMERA_rules_neg.xlsx
+++ b/inst/extdata/CAMERA_rules_neg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>name</t>
   </si>
@@ -455,6 +455,18 @@
   </si>
   <si>
     <t>[M-H-Hexose-H2O]-</t>
+  </si>
+  <si>
+    <t>[M+H-Hexose-H2O-CH4]+</t>
+  </si>
+  <si>
+    <t>[M+H-Hexose-H2O-CH3OH]+</t>
+  </si>
+  <si>
+    <t>[M+H-Hexose-H2O-C2H4O]+</t>
+  </si>
+  <si>
+    <t>[M+H-Hexose-H2O-C2H4O2]+</t>
   </si>
 </sst>
 </file>
@@ -941,11 +953,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D140" sqref="D140"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4176,6 +4188,102 @@
         <v>0.75</v>
       </c>
     </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A140" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B140" s="15">
+        <v>1</v>
+      </c>
+      <c r="C140" s="15">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <f>D139+D79+1.0073</f>
+        <v>-179.09138213500003</v>
+      </c>
+      <c r="E140" s="15">
+        <v>174</v>
+      </c>
+      <c r="F140" s="15">
+        <v>0</v>
+      </c>
+      <c r="G140" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B141" s="15">
+        <v>1</v>
+      </c>
+      <c r="C141" s="15">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <f>D139+D82+1.0073</f>
+        <v>-195.08629676500001</v>
+      </c>
+      <c r="E141" s="15">
+        <v>175</v>
+      </c>
+      <c r="F141" s="15">
+        <v>0</v>
+      </c>
+      <c r="G141" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A142" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B142" s="15">
+        <v>1</v>
+      </c>
+      <c r="C142" s="15">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <f>D139+D69+1.0073</f>
+        <v>-207.08629676500001</v>
+      </c>
+      <c r="E142" s="15">
+        <v>176</v>
+      </c>
+      <c r="F142" s="15">
+        <v>0</v>
+      </c>
+      <c r="G142" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B143" s="15">
+        <v>1</v>
+      </c>
+      <c r="C143" s="15">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <f>D139+D98+1.0073</f>
+        <v>-223.08121231000001</v>
+      </c>
+      <c r="E143" s="15">
+        <v>177</v>
+      </c>
+      <c r="F143" s="15">
+        <v>0</v>
+      </c>
+      <c r="G143" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
marked more as quasi ions
</commit_message>
<xml_diff>
--- a/inst/extdata/CAMERA_rules_neg.xlsx
+++ b/inst/extdata/CAMERA_rules_neg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmh331\Desktop\gits\common_mz\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmh331\Desktop\gits\commonMZ\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10650"/>
   </bookViews>
   <sheets>
     <sheet name="rules_jan_neg" sheetId="1" r:id="rId1"/>
@@ -956,17 +956,16 @@
   <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B138" sqref="B138"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.81640625"/>
-    <col min="2" max="1025" width="9.1796875"/>
+    <col min="1" max="1" width="35.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1058,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1264,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1282,13 +1281,13 @@
         <v>4</v>
       </c>
       <c r="F14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1380,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>30</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
@@ -1564,7 +1563,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>33</v>
       </c>
@@ -1610,7 +1609,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
@@ -1656,7 +1655,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>36</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -1725,7 +1724,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>39</v>
       </c>
@@ -1748,7 +1747,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>40</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>41</v>
       </c>
@@ -1794,7 +1793,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -1811,13 +1810,13 @@
         <v>13</v>
       </c>
       <c r="F37" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="12">
         <v>0.75</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1840,7 +1839,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>52</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>53</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>54</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>55</v>
       </c>
@@ -2125,7 +2124,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
         <v>56</v>
       </c>
@@ -2148,7 +2147,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
         <v>57</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>58</v>
       </c>
@@ -2188,13 +2187,13 @@
         <v>87</v>
       </c>
       <c r="F53" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="15">
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>59</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>60</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>61</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
         <v>62</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>63</v>
       </c>
@@ -2309,7 +2308,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
         <v>64</v>
       </c>
@@ -2332,7 +2331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
         <v>65</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
         <v>66</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>67</v>
       </c>
@@ -2401,7 +2400,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>68</v>
       </c>
@@ -2424,7 +2423,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
         <v>69</v>
       </c>
@@ -2447,7 +2446,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>70</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>71</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
         <v>72</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>73</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
         <v>74</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>75</v>
       </c>
@@ -2585,7 +2584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
         <v>76</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
         <v>77</v>
       </c>
@@ -2631,7 +2630,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
         <v>78</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>79</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
         <v>80</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
         <v>81</v>
       </c>
@@ -2723,7 +2722,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
         <v>82</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
         <v>83</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
         <v>84</v>
       </c>
@@ -2792,7 +2791,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
         <v>85</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
         <v>86</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
         <v>87</v>
       </c>
@@ -2861,7 +2860,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
         <v>88</v>
       </c>
@@ -2884,7 +2883,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
         <v>89</v>
       </c>
@@ -2907,7 +2906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
         <v>90</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
         <v>91</v>
       </c>
@@ -2955,7 +2954,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
         <v>92</v>
       </c>
@@ -2979,7 +2978,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
         <v>93</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
         <v>94</v>
       </c>
@@ -3027,7 +3026,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
         <v>95</v>
       </c>
@@ -3051,7 +3050,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
         <v>96</v>
       </c>
@@ -3075,7 +3074,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
         <v>97</v>
       </c>
@@ -3099,7 +3098,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>98</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>99</v>
       </c>
@@ -3147,7 +3146,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
         <v>100</v>
       </c>
@@ -3171,7 +3170,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
         <v>101</v>
       </c>
@@ -3195,7 +3194,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
         <v>102</v>
       </c>
@@ -3219,7 +3218,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
         <v>103</v>
       </c>
@@ -3243,7 +3242,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
         <v>104</v>
       </c>
@@ -3267,7 +3266,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
         <v>105</v>
       </c>
@@ -3290,7 +3289,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
         <v>106</v>
       </c>
@@ -3313,7 +3312,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
         <v>107</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
         <v>108</v>
       </c>
@@ -3359,7 +3358,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
         <v>109</v>
       </c>
@@ -3382,7 +3381,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
         <v>110</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
         <v>111</v>
       </c>
@@ -3428,7 +3427,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
         <v>112</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
         <v>113</v>
       </c>
@@ -3474,7 +3473,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
         <v>114</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>115</v>
       </c>
@@ -3520,7 +3519,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="15" t="s">
         <v>116</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>117</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
         <v>118</v>
       </c>
@@ -3589,7 +3588,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
         <v>119</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
         <v>120</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
         <v>121</v>
       </c>
@@ -3658,7 +3657,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>122</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
         <v>123</v>
       </c>
@@ -3704,7 +3703,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
         <v>124</v>
       </c>
@@ -3727,7 +3726,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
         <v>125</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
         <v>126</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
         <v>127</v>
       </c>
@@ -3796,7 +3795,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
         <v>128</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
         <v>129</v>
       </c>
@@ -3842,7 +3841,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
         <v>130</v>
       </c>
@@ -3865,7 +3864,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
         <v>131</v>
       </c>
@@ -3888,7 +3887,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
         <v>132</v>
       </c>
@@ -3911,7 +3910,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
         <v>133</v>
       </c>
@@ -3934,7 +3933,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
         <v>134</v>
       </c>
@@ -3957,7 +3956,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>135</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
         <v>136</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
         <v>137</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
         <v>138</v>
       </c>
@@ -4049,7 +4048,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
         <v>139</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
         <v>140</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
         <v>141</v>
       </c>
@@ -4118,7 +4117,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
         <v>142</v>
       </c>
@@ -4141,7 +4140,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
         <v>143</v>
       </c>
@@ -4164,7 +4163,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
         <v>144</v>
       </c>
@@ -4188,7 +4187,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
         <v>145</v>
       </c>
@@ -4212,7 +4211,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
         <v>146</v>
       </c>
@@ -4236,7 +4235,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
         <v>147</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
added loss of two hexoses. also fixed some copy pasting where negative mode was annotated as positive
</commit_message>
<xml_diff>
--- a/inst/extdata/CAMERA_rules_neg.xlsx
+++ b/inst/extdata/CAMERA_rules_neg.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>name</t>
   </si>
@@ -457,16 +457,19 @@
     <t>[M-H-Hexose-H2O]-</t>
   </si>
   <si>
-    <t>[M+H-Hexose-H2O-CH4]+</t>
-  </si>
-  <si>
-    <t>[M+H-Hexose-H2O-CH3OH]+</t>
-  </si>
-  <si>
-    <t>[M+H-Hexose-H2O-C2H4O]+</t>
-  </si>
-  <si>
-    <t>[M+H-Hexose-H2O-C2H4O2]+</t>
+    <t>[M-H-Hexose-H2O-CH4]-</t>
+  </si>
+  <si>
+    <t>[M-H-Hexose-H2O-CH3OH]-</t>
+  </si>
+  <si>
+    <t>[M-H-Hexose-H2O-C2H4O]-</t>
+  </si>
+  <si>
+    <t>[M-H-Hexose-H2O-C2H4O2]-</t>
+  </si>
+  <si>
+    <t>[M-H-(Hexose-H2O)2]-</t>
   </si>
 </sst>
 </file>
@@ -953,11 +956,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,6 +4286,30 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B144" s="15">
+        <v>1</v>
+      </c>
+      <c r="C144" s="15">
+        <v>1</v>
+      </c>
+      <c r="D144">
+        <f>-(2*162.05283-D2)</f>
+        <v>-325.11293645500001</v>
+      </c>
+      <c r="E144" s="15">
+        <v>178</v>
+      </c>
+      <c r="F144" s="15">
+        <v>0</v>
+      </c>
+      <c r="G144" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
acetyl and CH3 added
</commit_message>
<xml_diff>
--- a/inst/extdata/CAMERA_rules_neg.xlsx
+++ b/inst/extdata/CAMERA_rules_neg.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmh331\Desktop\gits\commonMZ\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55B1755-179E-4042-9B17-3FAC5340FE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rules_jan_neg" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>name</t>
   </si>
@@ -470,12 +484,18 @@
   </si>
   <si>
     <t>[M-H-(Hexose-H2O)2]-</t>
+  </si>
+  <si>
+    <t>[M-H-acetyl]-</t>
+  </si>
+  <si>
+    <t>[M-H-CH3]-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -591,23 +611,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,20 +974,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G146"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A147" sqref="A147"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875"/>
+    <col min="1" max="1" width="35.88671875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1037,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1083,7 +1102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1106,7 +1125,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1148,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1171,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1175,7 +1194,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1198,7 +1217,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1221,7 +1240,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -1244,7 +1263,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -1267,7 +1286,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
@@ -1290,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1313,7 +1332,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1355,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
@@ -1359,7 +1378,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1382,7 +1401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1405,7 +1424,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1428,7 +1447,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
@@ -1451,7 +1470,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
@@ -1474,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>28</v>
       </c>
@@ -1497,7 +1516,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -1520,7 +1539,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>30</v>
       </c>
@@ -1543,7 +1562,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1585,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
@@ -1589,7 +1608,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>33</v>
       </c>
@@ -1612,7 +1631,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>34</v>
       </c>
@@ -1635,7 +1654,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
@@ -1658,7 +1677,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1700,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1723,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -1727,7 +1746,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>39</v>
       </c>
@@ -1750,7 +1769,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>40</v>
       </c>
@@ -1773,7 +1792,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>41</v>
       </c>
@@ -1796,7 +1815,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>42</v>
       </c>
@@ -1819,7 +1838,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -1842,7 +1861,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1865,7 +1884,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>45</v>
       </c>
@@ -1888,7 +1907,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>46</v>
       </c>
@@ -1912,7 +1931,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1936,7 +1955,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>48</v>
       </c>
@@ -1960,7 +1979,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -1984,7 +2003,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>50</v>
       </c>
@@ -2008,7 +2027,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>51</v>
       </c>
@@ -2032,2281 +2051,2329 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="13">
-        <v>1</v>
-      </c>
-      <c r="C47" s="13">
-        <v>-1</v>
-      </c>
-      <c r="D47" s="13">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>-1</v>
+      </c>
+      <c r="D47">
         <f>57.95862042+D2</f>
         <v>56.951343965</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47">
         <v>23</v>
       </c>
-      <c r="F47" s="13">
-        <v>0</v>
-      </c>
-      <c r="G47" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="13">
-        <v>1</v>
-      </c>
-      <c r="C48" s="13">
-        <v>-1</v>
-      </c>
-      <c r="D48" s="13">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>-1</v>
+      </c>
+      <c r="D48">
         <f>115.9172408+D2</f>
         <v>114.90996434500001</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48">
         <v>24</v>
       </c>
-      <c r="F48" s="13">
-        <v>0</v>
-      </c>
-      <c r="G48" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="13">
-        <v>1</v>
-      </c>
-      <c r="C49" s="13">
-        <v>-1</v>
-      </c>
-      <c r="D49" s="13">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>-1</v>
+      </c>
+      <c r="D49">
         <f>73.93256012+D2</f>
         <v>72.925283665000009</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49">
         <v>25</v>
       </c>
-      <c r="F49" s="13">
-        <v>0</v>
-      </c>
-      <c r="G49" s="13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="14">
-        <v>1</v>
-      </c>
-      <c r="C50" s="14">
-        <v>-1</v>
-      </c>
-      <c r="D50" s="14">
+      <c r="B50" s="13">
+        <v>1</v>
+      </c>
+      <c r="C50" s="13">
+        <v>-1</v>
+      </c>
+      <c r="D50" s="13">
         <v>39.02402309</v>
       </c>
-      <c r="E50" s="14">
+      <c r="E50" s="13">
         <v>26</v>
       </c>
-      <c r="F50" s="14">
-        <v>0</v>
-      </c>
-      <c r="G50" s="14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="F50" s="13">
+        <v>0</v>
+      </c>
+      <c r="G50" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="15">
-        <v>1</v>
-      </c>
-      <c r="C51" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D51" s="15">
+      <c r="B51" s="14">
+        <v>1</v>
+      </c>
+      <c r="C51" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D51" s="14">
         <v>-47.012754870000002</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="14">
         <v>85</v>
       </c>
-      <c r="F51" s="15">
-        <v>0</v>
-      </c>
-      <c r="G51" s="15">
+      <c r="F51" s="14">
+        <v>0</v>
+      </c>
+      <c r="G51" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="15">
-        <v>1</v>
-      </c>
-      <c r="C52" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D52" s="15">
+      <c r="B52" s="14">
+        <v>1</v>
+      </c>
+      <c r="C52" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D52" s="14">
         <v>-18.03382465</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="14">
         <v>86</v>
       </c>
-      <c r="F52" s="15">
-        <v>0</v>
-      </c>
-      <c r="G52" s="15">
+      <c r="F52" s="14">
+        <v>0</v>
+      </c>
+      <c r="G52" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="15" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="15">
-        <v>1</v>
-      </c>
-      <c r="C53" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D53" s="15">
+      <c r="B53" s="14">
+        <v>1</v>
+      </c>
+      <c r="C53" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D53" s="14">
         <v>-19.017840240000002</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="14">
         <v>87</v>
       </c>
-      <c r="F53" s="15">
-        <v>1</v>
-      </c>
-      <c r="G53" s="15">
+      <c r="F53" s="14">
+        <v>1</v>
+      </c>
+      <c r="G53" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B54" s="15">
-        <v>1</v>
-      </c>
-      <c r="C54" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D54" s="15">
+      <c r="B54" s="14">
+        <v>1</v>
+      </c>
+      <c r="C54" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D54" s="14">
         <v>-43.017840239999998</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="14">
         <v>88</v>
       </c>
-      <c r="F54" s="15">
-        <v>0</v>
-      </c>
-      <c r="G54" s="15">
+      <c r="F54" s="14">
+        <v>0</v>
+      </c>
+      <c r="G54" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="15">
-        <v>1</v>
-      </c>
-      <c r="C55" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D55" s="15">
+      <c r="B55" s="14">
+        <v>1</v>
+      </c>
+      <c r="C55" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D55" s="14">
         <v>-44.997104800000002</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="14">
         <v>89</v>
       </c>
-      <c r="F55" s="15">
-        <v>0</v>
-      </c>
-      <c r="G55" s="15">
+      <c r="F55" s="14">
+        <v>0</v>
+      </c>
+      <c r="G55" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="15">
-        <v>1</v>
-      </c>
-      <c r="C56" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D56" s="15">
+      <c r="B56" s="14">
+        <v>1</v>
+      </c>
+      <c r="C56" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D56" s="14">
         <v>-62.02365391</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="14">
         <v>90</v>
       </c>
-      <c r="F56" s="15">
-        <v>0</v>
-      </c>
-      <c r="G56" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+      <c r="F56" s="14">
+        <v>0</v>
+      </c>
+      <c r="G56" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B57" s="15">
-        <v>1</v>
-      </c>
-      <c r="C57" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D57" s="15">
+      <c r="B57" s="14">
+        <v>1</v>
+      </c>
+      <c r="C57" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D57" s="14">
         <v>-64.03930398</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="14">
         <v>91</v>
       </c>
-      <c r="F57" s="15">
-        <v>0</v>
-      </c>
-      <c r="G57" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="F57" s="14">
+        <v>0</v>
+      </c>
+      <c r="G57" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="15">
-        <v>1</v>
-      </c>
-      <c r="C58" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D58" s="15">
+      <c r="B58" s="14">
+        <v>1</v>
+      </c>
+      <c r="C58" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D58" s="14">
         <v>-36.044389350000003</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="14">
         <v>92</v>
       </c>
-      <c r="F58" s="15">
-        <v>0</v>
-      </c>
-      <c r="G58" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="F58" s="14">
+        <v>0</v>
+      </c>
+      <c r="G58" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B59" s="15">
-        <v>1</v>
-      </c>
-      <c r="C59" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D59" s="15">
+      <c r="B59" s="14">
+        <v>1</v>
+      </c>
+      <c r="C59" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D59" s="14">
         <v>-60.044389350000003</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="14">
         <v>93</v>
       </c>
-      <c r="F59" s="15">
-        <v>0</v>
-      </c>
-      <c r="G59" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="F59" s="14">
+        <v>0</v>
+      </c>
+      <c r="G59" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B60" s="15">
-        <v>1</v>
-      </c>
-      <c r="C60" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D60" s="15">
+      <c r="B60" s="14">
+        <v>1</v>
+      </c>
+      <c r="C60" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D60" s="14">
         <v>-32.979346239999998</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="14">
         <v>94</v>
       </c>
-      <c r="F60" s="15">
-        <v>0</v>
-      </c>
-      <c r="G60" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="F60" s="14">
+        <v>0</v>
+      </c>
+      <c r="G60" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B61" s="15">
-        <v>1</v>
-      </c>
-      <c r="C61" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D61" s="15">
+      <c r="B61" s="14">
+        <v>1</v>
+      </c>
+      <c r="C61" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D61" s="14">
         <v>-96.011374680000003</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="14">
         <v>95</v>
       </c>
-      <c r="F61" s="15">
-        <v>0</v>
-      </c>
-      <c r="G61" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="F61" s="14">
+        <v>0</v>
+      </c>
+      <c r="G61" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="15">
-        <v>1</v>
-      </c>
-      <c r="C62" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D62" s="15">
+      <c r="B62" s="14">
+        <v>1</v>
+      </c>
+      <c r="C62" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D62" s="14">
         <v>-37.028404940000001</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="14">
         <v>96</v>
       </c>
-      <c r="F62" s="15">
-        <v>0</v>
-      </c>
-      <c r="G62" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+      <c r="F62" s="14">
+        <v>0</v>
+      </c>
+      <c r="G62" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B63" s="15">
-        <v>1</v>
-      </c>
-      <c r="C63" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D63" s="15">
+      <c r="B63" s="14">
+        <v>1</v>
+      </c>
+      <c r="C63" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D63" s="14">
         <v>-15.02292561</v>
       </c>
-      <c r="E63" s="15">
+      <c r="E63" s="14">
         <v>97</v>
       </c>
-      <c r="F63" s="15">
-        <v>0</v>
-      </c>
-      <c r="G63" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="F63" s="14">
+        <v>0</v>
+      </c>
+      <c r="G63" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="15">
-        <v>1</v>
-      </c>
-      <c r="C64" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D64" s="15">
+      <c r="B64" s="14">
+        <v>1</v>
+      </c>
+      <c r="C64" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D64" s="14">
         <v>-17.002190169999999</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="14">
         <v>98</v>
       </c>
-      <c r="F64" s="15">
-        <v>0</v>
-      </c>
-      <c r="G64" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="F64" s="14">
+        <v>0</v>
+      </c>
+      <c r="G64" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="15">
-        <v>1</v>
-      </c>
-      <c r="C65" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D65" s="15">
+      <c r="B65" s="14">
+        <v>1</v>
+      </c>
+      <c r="C65" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D65" s="14">
         <v>-27.022925610000001</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E65" s="14">
         <v>99</v>
       </c>
-      <c r="F65" s="15">
-        <v>0</v>
-      </c>
-      <c r="G65" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="F65" s="14">
+        <v>0</v>
+      </c>
+      <c r="G65" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="15">
-        <v>1</v>
-      </c>
-      <c r="C66" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D66" s="15">
+      <c r="B66" s="14">
+        <v>1</v>
+      </c>
+      <c r="C66" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D66" s="14">
         <v>-29.038575680000001</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="14">
         <v>100</v>
       </c>
-      <c r="F66" s="15">
-        <v>0</v>
-      </c>
-      <c r="G66" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+      <c r="F66" s="14">
+        <v>0</v>
+      </c>
+      <c r="G66" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="15">
-        <v>1</v>
-      </c>
-      <c r="C67" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D67" s="15">
+      <c r="B67" s="14">
+        <v>1</v>
+      </c>
+      <c r="C67" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D67" s="14">
         <v>-29.002190169999999</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="14">
         <v>101</v>
       </c>
-      <c r="F67" s="15">
-        <v>0</v>
-      </c>
-      <c r="G67" s="15">
+      <c r="F67" s="14">
+        <v>0</v>
+      </c>
+      <c r="G67" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="15">
-        <v>1</v>
-      </c>
-      <c r="C68" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D68" s="15">
+      <c r="B68" s="14">
+        <v>1</v>
+      </c>
+      <c r="C68" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D68" s="14">
         <v>-43.054225750000001</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E68" s="14">
         <v>102</v>
       </c>
-      <c r="F68" s="15">
-        <v>0</v>
-      </c>
-      <c r="G68" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+      <c r="F68" s="14">
+        <v>0</v>
+      </c>
+      <c r="G68" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B69" s="15">
-        <v>1</v>
-      </c>
-      <c r="C69" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D69" s="15">
+      <c r="B69" s="14">
+        <v>1</v>
+      </c>
+      <c r="C69" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D69" s="14">
         <v>-45.033490309999998</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="14">
         <v>103</v>
       </c>
-      <c r="F69" s="15">
-        <v>0</v>
-      </c>
-      <c r="G69" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+      <c r="F69" s="14">
+        <v>0</v>
+      </c>
+      <c r="G69" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="15">
-        <v>1</v>
-      </c>
-      <c r="C70" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D70" s="15">
+      <c r="B70" s="14">
+        <v>1</v>
+      </c>
+      <c r="C70" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D70" s="14">
         <v>-55.054225750000001</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="14">
         <v>104</v>
       </c>
-      <c r="F70" s="15">
-        <v>0</v>
-      </c>
-      <c r="G70" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="F70" s="14">
+        <v>0</v>
+      </c>
+      <c r="G70" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="15">
-        <v>1</v>
-      </c>
-      <c r="C71" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D71" s="15">
+      <c r="B71" s="14">
+        <v>1</v>
+      </c>
+      <c r="C71" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D71" s="14">
         <v>-57.033490309999998</v>
       </c>
-      <c r="E71" s="15">
+      <c r="E71" s="14">
         <v>105</v>
       </c>
-      <c r="F71" s="15">
-        <v>0</v>
-      </c>
-      <c r="G71" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="F71" s="14">
+        <v>0</v>
+      </c>
+      <c r="G71" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="15">
-        <v>1</v>
-      </c>
-      <c r="C72" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D72" s="15">
+      <c r="B72" s="14">
+        <v>1</v>
+      </c>
+      <c r="C72" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D72" s="14">
         <v>-57.06987582</v>
       </c>
-      <c r="E72" s="15">
+      <c r="E72" s="14">
         <v>106</v>
       </c>
-      <c r="F72" s="15">
-        <v>0</v>
-      </c>
-      <c r="G72" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="F72" s="14">
+        <v>0</v>
+      </c>
+      <c r="G72" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="15">
-        <v>1</v>
-      </c>
-      <c r="C73" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D73" s="15">
+      <c r="B73" s="14">
+        <v>1</v>
+      </c>
+      <c r="C73" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D73" s="14">
         <v>-69.069875819999993</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E73" s="14">
         <v>107</v>
       </c>
-      <c r="F73" s="15">
-        <v>0</v>
-      </c>
-      <c r="G73" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="F73" s="14">
+        <v>0</v>
+      </c>
+      <c r="G73" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="15">
-        <v>1</v>
-      </c>
-      <c r="C74" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D74" s="15">
+      <c r="B74" s="14">
+        <v>1</v>
+      </c>
+      <c r="C74" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D74" s="14">
         <v>-71.049140379999997</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="14">
         <v>108</v>
       </c>
-      <c r="F74" s="15">
-        <v>0</v>
-      </c>
-      <c r="G74" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="F74" s="14">
+        <v>0</v>
+      </c>
+      <c r="G74" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="B75" s="15">
-        <v>1</v>
-      </c>
-      <c r="C75" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D75" s="15">
+      <c r="B75" s="14">
+        <v>1</v>
+      </c>
+      <c r="C75" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D75" s="14">
         <v>-71.08552589</v>
       </c>
-      <c r="E75" s="15">
+      <c r="E75" s="14">
         <v>109</v>
       </c>
-      <c r="F75" s="15">
-        <v>0</v>
-      </c>
-      <c r="G75" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+      <c r="F75" s="14">
+        <v>0</v>
+      </c>
+      <c r="G75" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="15">
-        <v>1</v>
-      </c>
-      <c r="C76" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D76" s="15">
+      <c r="B76" s="14">
+        <v>1</v>
+      </c>
+      <c r="C76" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D76" s="14">
         <v>-85.101175960000006</v>
       </c>
-      <c r="E76" s="15">
+      <c r="E76" s="14">
         <v>110</v>
       </c>
-      <c r="F76" s="15">
-        <v>0</v>
-      </c>
-      <c r="G76" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+      <c r="F76" s="14">
+        <v>0</v>
+      </c>
+      <c r="G76" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B77" s="15">
-        <v>1</v>
-      </c>
-      <c r="C77" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D77" s="15">
+      <c r="B77" s="14">
+        <v>1</v>
+      </c>
+      <c r="C77" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D77" s="14">
         <v>-89.059705080000001</v>
       </c>
-      <c r="E77" s="15">
+      <c r="E77" s="14">
         <v>111</v>
       </c>
-      <c r="F77" s="15">
-        <v>0</v>
-      </c>
-      <c r="G77" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+      <c r="F77" s="14">
+        <v>0</v>
+      </c>
+      <c r="G77" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="B78" s="15">
-        <v>1</v>
-      </c>
-      <c r="C78" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D78" s="15">
+      <c r="B78" s="14">
+        <v>1</v>
+      </c>
+      <c r="C78" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D78" s="14">
         <v>-65.023319569999998</v>
       </c>
-      <c r="E78" s="15">
+      <c r="E78" s="14">
         <v>112</v>
       </c>
-      <c r="F78" s="15">
-        <v>0</v>
-      </c>
-      <c r="G78" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+      <c r="F78" s="14">
+        <v>0</v>
+      </c>
+      <c r="G78" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="15">
-        <v>1</v>
-      </c>
-      <c r="C79" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D79" s="15">
+      <c r="B79" s="14">
+        <v>1</v>
+      </c>
+      <c r="C79" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D79" s="14">
         <v>-17.038575680000001</v>
       </c>
-      <c r="E79" s="15">
+      <c r="E79" s="14">
         <v>113</v>
       </c>
-      <c r="F79" s="15">
-        <v>0</v>
-      </c>
-      <c r="G79" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+      <c r="F79" s="14">
+        <v>0</v>
+      </c>
+      <c r="G79" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="15">
-        <v>1</v>
-      </c>
-      <c r="C80" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D80" s="15">
+      <c r="B80" s="14">
+        <v>1</v>
+      </c>
+      <c r="C80" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D80" s="14">
         <v>-31.017840240000002</v>
       </c>
-      <c r="E80" s="15">
+      <c r="E80" s="14">
         <v>114</v>
       </c>
-      <c r="F80" s="15">
-        <v>0</v>
-      </c>
-      <c r="G80" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+      <c r="F80" s="14">
+        <v>0</v>
+      </c>
+      <c r="G80" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="15">
-        <v>1</v>
-      </c>
-      <c r="C81" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D81" s="15">
+      <c r="B81" s="14">
+        <v>1</v>
+      </c>
+      <c r="C81" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D81" s="14">
         <v>-31.054225750000001</v>
       </c>
-      <c r="E81" s="15">
+      <c r="E81" s="14">
         <v>115</v>
       </c>
-      <c r="F81" s="15">
-        <v>0</v>
-      </c>
-      <c r="G81" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+      <c r="F81" s="14">
+        <v>0</v>
+      </c>
+      <c r="G81" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="15">
-        <v>1</v>
-      </c>
-      <c r="C82" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D82" s="15">
+      <c r="B82" s="14">
+        <v>1</v>
+      </c>
+      <c r="C82" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D82" s="14">
         <v>-33.033490309999998</v>
       </c>
-      <c r="E82" s="15">
+      <c r="E82" s="14">
         <v>116</v>
       </c>
-      <c r="F82" s="15">
-        <v>0</v>
-      </c>
-      <c r="G82" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
+      <c r="F82" s="14">
+        <v>0</v>
+      </c>
+      <c r="G82" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B83" s="15">
-        <v>1</v>
-      </c>
-      <c r="C83" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D83" s="15">
+      <c r="B83" s="14">
+        <v>1</v>
+      </c>
+      <c r="C83" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D83" s="14">
         <v>-41.038575680000001</v>
       </c>
-      <c r="E83" s="15">
+      <c r="E83" s="14">
         <v>117</v>
       </c>
-      <c r="F83" s="15">
-        <v>0</v>
-      </c>
-      <c r="G83" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+      <c r="F83" s="14">
+        <v>0</v>
+      </c>
+      <c r="G83" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B84" s="15">
-        <v>1</v>
-      </c>
-      <c r="C84" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D84" s="15">
+      <c r="B84" s="14">
+        <v>1</v>
+      </c>
+      <c r="C84" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D84" s="14">
         <v>-59.049140379999997</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="14">
         <v>118</v>
       </c>
-      <c r="F84" s="15">
-        <v>0</v>
-      </c>
-      <c r="G84" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
+      <c r="F84" s="14">
+        <v>0</v>
+      </c>
+      <c r="G84" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B85" s="15">
-        <v>1</v>
-      </c>
-      <c r="C85" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D85" s="15">
+      <c r="B85" s="14">
+        <v>1</v>
+      </c>
+      <c r="C85" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D85" s="14">
         <f>-86.03677947+D2</f>
         <v>-87.044055924999995</v>
       </c>
-      <c r="E85" s="15">
+      <c r="E85" s="14">
         <v>119</v>
       </c>
-      <c r="F85" s="15">
-        <v>0</v>
-      </c>
-      <c r="G85" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
+      <c r="F85" s="14">
+        <v>0</v>
+      </c>
+      <c r="G85" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B86" s="15">
-        <v>1</v>
-      </c>
-      <c r="C86" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D86" s="15">
+      <c r="B86" s="14">
+        <v>1</v>
+      </c>
+      <c r="C86" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D86" s="14">
         <f>-79.95681459+D2</f>
         <v>-80.964091044999989</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="14">
         <v>120</v>
       </c>
-      <c r="F86" s="15">
-        <v>0</v>
-      </c>
-      <c r="G86" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="F86" s="14">
+        <v>0</v>
+      </c>
+      <c r="G86" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B87" s="15">
-        <v>1</v>
-      </c>
-      <c r="C87" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D87" s="15">
+      <c r="B87" s="14">
+        <v>1</v>
+      </c>
+      <c r="C87" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D87" s="14">
         <f>-97.96737929+D2</f>
         <v>-98.974655744999993</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E87" s="14">
         <v>121</v>
       </c>
-      <c r="F87" s="15">
-        <v>0</v>
-      </c>
-      <c r="G87" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
+      <c r="F87" s="14">
+        <v>0</v>
+      </c>
+      <c r="G87" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B88" s="15">
-        <v>1</v>
-      </c>
-      <c r="C88" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D88" s="15">
+      <c r="B88" s="14">
+        <v>1</v>
+      </c>
+      <c r="C88" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D88" s="14">
         <f>-114.9939284+D2</f>
         <v>-116.001204855</v>
       </c>
-      <c r="E88" s="15">
+      <c r="E88" s="14">
         <v>122</v>
       </c>
-      <c r="F88" s="15">
-        <v>0</v>
-      </c>
-      <c r="G88" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
+      <c r="F88" s="14">
+        <v>0</v>
+      </c>
+      <c r="G88" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B89" s="15">
-        <v>1</v>
-      </c>
-      <c r="C89" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D89" s="15">
+      <c r="B89" s="14">
+        <v>1</v>
+      </c>
+      <c r="C89" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D89" s="14">
         <f>-57.05784925+D2</f>
         <v>-58.065125705</v>
       </c>
-      <c r="E89" s="15">
+      <c r="E89" s="14">
         <v>123</v>
       </c>
-      <c r="F89" s="15">
-        <v>0</v>
-      </c>
-      <c r="G89" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+      <c r="F89" s="14">
+        <v>0</v>
+      </c>
+      <c r="G89" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B90" s="15">
-        <v>1</v>
-      </c>
-      <c r="C90" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D90" s="15">
+      <c r="B90" s="14">
+        <v>1</v>
+      </c>
+      <c r="C90" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D90" s="14">
         <f>-62.00039396+D2</f>
         <v>-63.007670415</v>
       </c>
-      <c r="E90" s="15">
+      <c r="E90" s="14">
         <v>124</v>
       </c>
-      <c r="F90" s="15">
-        <v>0</v>
-      </c>
-      <c r="G90" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="15" t="s">
+      <c r="F90" s="14">
+        <v>0</v>
+      </c>
+      <c r="G90" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B91" s="15">
-        <v>1</v>
-      </c>
-      <c r="C91" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D91" s="15">
+      <c r="B91" s="14">
+        <v>1</v>
+      </c>
+      <c r="C91" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D91" s="14">
         <f>-80.04734417+D2</f>
         <v>-81.054620624999998</v>
       </c>
-      <c r="E91" s="15">
+      <c r="E91" s="14">
         <v>125</v>
       </c>
-      <c r="F91" s="15">
-        <v>0</v>
-      </c>
-      <c r="G91" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
+      <c r="F91" s="14">
+        <v>0</v>
+      </c>
+      <c r="G91" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B92" s="15">
-        <v>1</v>
-      </c>
-      <c r="C92" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D92" s="15">
+      <c r="B92" s="14">
+        <v>1</v>
+      </c>
+      <c r="C92" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D92" s="14">
         <f>-73.01637837+D2</f>
         <v>-74.023654824999994</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E92" s="14">
         <v>126</v>
       </c>
-      <c r="F92" s="15">
-        <v>0</v>
-      </c>
-      <c r="G92" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="15" t="s">
+      <c r="F92" s="14">
+        <v>0</v>
+      </c>
+      <c r="G92" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="B93" s="15">
-        <v>1</v>
-      </c>
-      <c r="C93" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D93" s="15">
+      <c r="B93" s="14">
+        <v>1</v>
+      </c>
+      <c r="C93" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D93" s="14">
         <f>-87.03202844+D2</f>
         <v>-88.039304895000001</v>
       </c>
-      <c r="E93" s="15">
+      <c r="E93" s="14">
         <v>127</v>
       </c>
-      <c r="F93" s="15">
-        <v>0</v>
-      </c>
-      <c r="G93" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="15" t="s">
+      <c r="F93" s="14">
+        <v>0</v>
+      </c>
+      <c r="G93" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B94" s="15">
-        <v>1</v>
-      </c>
-      <c r="C94" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D94" s="15">
+      <c r="B94" s="14">
+        <v>1</v>
+      </c>
+      <c r="C94" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D94" s="14">
         <f>-118.0418648+D2</f>
         <v>-119.04914125499999</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="14">
         <v>128</v>
       </c>
-      <c r="F94" s="15">
-        <v>0</v>
-      </c>
-      <c r="G94" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
+      <c r="F94" s="14">
+        <v>0</v>
+      </c>
+      <c r="G94" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="B95" s="15">
-        <v>1</v>
-      </c>
-      <c r="C95" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D95" s="15">
+      <c r="B95" s="14">
+        <v>1</v>
+      </c>
+      <c r="C95" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D95" s="14">
         <f>-135.0684139+D2</f>
         <v>-136.07569035500001</v>
       </c>
-      <c r="E95" s="15">
+      <c r="E95" s="14">
         <v>129</v>
       </c>
-      <c r="F95" s="15">
-        <v>0</v>
-      </c>
-      <c r="G95" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="15" t="s">
+      <c r="F95" s="14">
+        <v>0</v>
+      </c>
+      <c r="G95" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B96" s="15">
-        <v>1</v>
-      </c>
-      <c r="C96" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D96" s="15">
+      <c r="B96" s="14">
+        <v>1</v>
+      </c>
+      <c r="C96" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D96" s="14">
         <f>-136.0524295+D2</f>
         <v>-137.059705955</v>
       </c>
-      <c r="E96" s="15">
+      <c r="E96" s="14">
         <v>130</v>
       </c>
-      <c r="F96" s="15">
-        <v>0</v>
-      </c>
-      <c r="G96" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="15" t="s">
+      <c r="F96" s="14">
+        <v>0</v>
+      </c>
+      <c r="G96" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B97" s="15">
-        <v>1</v>
-      </c>
-      <c r="C97" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D97" s="15">
+      <c r="B97" s="14">
+        <v>1</v>
+      </c>
+      <c r="C97" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D97" s="14">
         <f>-58.00547933+D2</f>
         <v>-59.012755785000003</v>
       </c>
-      <c r="E97" s="15">
+      <c r="E97" s="14">
         <v>131</v>
       </c>
-      <c r="F97" s="15">
-        <v>0</v>
-      </c>
-      <c r="G97" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+      <c r="F97" s="14">
+        <v>0</v>
+      </c>
+      <c r="G97" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="B98" s="15">
-        <v>1</v>
-      </c>
-      <c r="C98" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D98" s="15">
+      <c r="B98" s="14">
+        <v>1</v>
+      </c>
+      <c r="C98" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D98" s="14">
         <f>-60.0211294+D2</f>
         <v>-61.028405855000003</v>
       </c>
-      <c r="E98" s="15">
+      <c r="E98" s="14">
         <v>132</v>
       </c>
-      <c r="F98" s="15">
-        <v>0</v>
-      </c>
-      <c r="G98" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+      <c r="F98" s="14">
+        <v>0</v>
+      </c>
+      <c r="G98" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="B99" s="15">
-        <v>1</v>
-      </c>
-      <c r="C99" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D99" s="15">
+      <c r="B99" s="14">
+        <v>1</v>
+      </c>
+      <c r="C99" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D99" s="14">
         <f>-84.05751491+D2</f>
         <v>-85.064791364999991</v>
       </c>
-      <c r="E99" s="15">
+      <c r="E99" s="14">
         <v>133</v>
       </c>
-      <c r="F99" s="15">
-        <v>0</v>
-      </c>
-      <c r="G99" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="15" t="s">
+      <c r="F99" s="14">
+        <v>0</v>
+      </c>
+      <c r="G99" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="15">
-        <v>1</v>
-      </c>
-      <c r="C100" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D100" s="15">
+      <c r="B100" s="14">
+        <v>1</v>
+      </c>
+      <c r="C100" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D100" s="14">
         <v>-92.034219522000001</v>
       </c>
-      <c r="E100" s="15">
+      <c r="E100" s="14">
         <v>134</v>
       </c>
-      <c r="F100" s="15">
-        <v>0</v>
-      </c>
-      <c r="G100" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
+      <c r="F100" s="14">
+        <v>0</v>
+      </c>
+      <c r="G100" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B101" s="15">
-        <v>1</v>
-      </c>
-      <c r="C101" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D101" s="15">
+      <c r="B101" s="14">
+        <v>1</v>
+      </c>
+      <c r="C101" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D101" s="14">
         <v>-97.060768628999995</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="14">
         <v>135</v>
       </c>
-      <c r="F101" s="15">
-        <v>0</v>
-      </c>
-      <c r="G101" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="15" t="s">
+      <c r="F101" s="14">
+        <v>0</v>
+      </c>
+      <c r="G101" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="15">
-        <v>1</v>
-      </c>
-      <c r="C102" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D102" s="15">
+      <c r="B102" s="14">
+        <v>1</v>
+      </c>
+      <c r="C102" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D102" s="14">
         <v>-118.04986959199999</v>
       </c>
-      <c r="E102" s="15">
+      <c r="E102" s="14">
         <v>136</v>
       </c>
-      <c r="F102" s="15">
-        <v>0</v>
-      </c>
-      <c r="G102" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="15" t="s">
+      <c r="F102" s="14">
+        <v>0</v>
+      </c>
+      <c r="G102" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B103" s="15">
-        <v>1</v>
-      </c>
-      <c r="C103" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D103" s="15">
+      <c r="B103" s="14">
+        <v>1</v>
+      </c>
+      <c r="C103" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D103" s="14">
         <v>-130.086255102</v>
       </c>
-      <c r="E103" s="15">
+      <c r="E103" s="14">
         <v>137</v>
       </c>
-      <c r="F103" s="15">
-        <v>0</v>
-      </c>
-      <c r="G103" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
+      <c r="F103" s="14">
+        <v>0</v>
+      </c>
+      <c r="G103" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="B104" s="15">
-        <v>1</v>
-      </c>
-      <c r="C104" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D104" s="15">
+      <c r="B104" s="14">
+        <v>1</v>
+      </c>
+      <c r="C104" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D104" s="14">
         <v>-93.018235114999996</v>
       </c>
-      <c r="E104" s="15">
+      <c r="E104" s="14">
         <v>138</v>
       </c>
-      <c r="F104" s="15">
-        <v>0</v>
-      </c>
-      <c r="G104" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="15" t="s">
+      <c r="F104" s="14">
+        <v>0</v>
+      </c>
+      <c r="G104" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B105" s="15">
-        <v>1</v>
-      </c>
-      <c r="C105" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D105" s="15">
+      <c r="B105" s="14">
+        <v>1</v>
+      </c>
+      <c r="C105" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D105" s="14">
         <v>-73.028405855000003</v>
       </c>
-      <c r="E105" s="15">
+      <c r="E105" s="14">
         <v>139</v>
       </c>
-      <c r="F105" s="15">
-        <v>0</v>
-      </c>
-      <c r="G105" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="15" t="s">
+      <c r="F105" s="14">
+        <v>0</v>
+      </c>
+      <c r="G105" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B106" s="15">
-        <v>1</v>
-      </c>
-      <c r="C106" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D106" s="15">
+      <c r="B106" s="14">
+        <v>1</v>
+      </c>
+      <c r="C106" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D106" s="14">
         <v>-75.044055924999995</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106" s="14">
         <v>140</v>
       </c>
-      <c r="F106" s="15">
-        <v>0</v>
-      </c>
-      <c r="G106" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="15" t="s">
+      <c r="F106" s="14">
+        <v>0</v>
+      </c>
+      <c r="G106" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B107" s="15">
-        <v>1</v>
-      </c>
-      <c r="C107" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D107" s="15">
+      <c r="B107" s="14">
+        <v>1</v>
+      </c>
+      <c r="C107" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D107" s="14">
         <v>-54.054954961999996</v>
       </c>
-      <c r="E107" s="15">
+      <c r="E107" s="14">
         <v>141</v>
       </c>
-      <c r="F107" s="15">
-        <v>0</v>
-      </c>
-      <c r="G107" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="15" t="s">
+      <c r="F107" s="14">
+        <v>0</v>
+      </c>
+      <c r="G107" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="15">
-        <v>1</v>
-      </c>
-      <c r="C108" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D108" s="15">
+      <c r="B108" s="14">
+        <v>1</v>
+      </c>
+      <c r="C108" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D108" s="14">
         <v>-77.023320484999999</v>
       </c>
-      <c r="E108" s="15">
+      <c r="E108" s="14">
         <v>142</v>
       </c>
-      <c r="F108" s="15">
-        <v>0</v>
-      </c>
-      <c r="G108" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="15" t="s">
+      <c r="F108" s="14">
+        <v>0</v>
+      </c>
+      <c r="G108" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="B109" s="15">
-        <v>1</v>
-      </c>
-      <c r="C109" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D109" s="15">
+      <c r="B109" s="14">
+        <v>1</v>
+      </c>
+      <c r="C109" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D109" s="14">
         <v>-99.080441434999997</v>
       </c>
-      <c r="E109" s="15">
+      <c r="E109" s="14">
         <v>143</v>
       </c>
-      <c r="F109" s="15">
-        <v>0</v>
-      </c>
-      <c r="G109" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="15" t="s">
+      <c r="F109" s="14">
+        <v>0</v>
+      </c>
+      <c r="G109" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B110" s="15">
-        <v>1</v>
-      </c>
-      <c r="C110" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D110" s="15">
+      <c r="B110" s="14">
+        <v>1</v>
+      </c>
+      <c r="C110" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D110" s="14">
         <v>-75.091674808999997</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="14">
         <v>144</v>
       </c>
-      <c r="F110" s="15">
-        <v>0</v>
-      </c>
-      <c r="G110" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="15" t="s">
+      <c r="F110" s="14">
+        <v>0</v>
+      </c>
+      <c r="G110" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B111" s="15">
-        <v>1</v>
-      </c>
-      <c r="C111" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D111" s="15">
+      <c r="B111" s="14">
+        <v>1</v>
+      </c>
+      <c r="C111" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D111" s="14">
         <v>-93.054620624999998</v>
       </c>
-      <c r="E111" s="15">
+      <c r="E111" s="14">
         <v>145</v>
       </c>
-      <c r="F111" s="15">
-        <v>0</v>
-      </c>
-      <c r="G111" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="15" t="s">
+      <c r="F111" s="14">
+        <v>0</v>
+      </c>
+      <c r="G111" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B112" s="15">
-        <v>1</v>
-      </c>
-      <c r="C112" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D112" s="15">
+      <c r="B112" s="14">
+        <v>1</v>
+      </c>
+      <c r="C112" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D112" s="14">
         <v>-91.075356064999994</v>
       </c>
-      <c r="E112" s="15">
+      <c r="E112" s="14">
         <v>146</v>
       </c>
-      <c r="F112" s="15">
-        <v>0</v>
-      </c>
-      <c r="G112" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="15" t="s">
+      <c r="F112" s="14">
+        <v>0</v>
+      </c>
+      <c r="G112" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B113" s="15">
-        <v>1</v>
-      </c>
-      <c r="C113" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D113" s="15">
+      <c r="B113" s="14">
+        <v>1</v>
+      </c>
+      <c r="C113" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D113" s="14">
         <v>-158.08116973200001</v>
       </c>
-      <c r="E113" s="15">
+      <c r="E113" s="14">
         <v>147</v>
       </c>
-      <c r="F113" s="15">
-        <v>0</v>
-      </c>
-      <c r="G113" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="15" t="s">
+      <c r="F113" s="14">
+        <v>0</v>
+      </c>
+      <c r="G113" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B114" s="15">
-        <v>1</v>
-      </c>
-      <c r="C114" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D114" s="15">
+      <c r="B114" s="14">
+        <v>1</v>
+      </c>
+      <c r="C114" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D114" s="14">
         <v>-73.064791365000005</v>
       </c>
-      <c r="E114" s="15">
+      <c r="E114" s="14">
         <v>148</v>
       </c>
-      <c r="F114" s="15">
-        <v>0</v>
-      </c>
-      <c r="G114" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="15" t="s">
+      <c r="F114" s="14">
+        <v>0</v>
+      </c>
+      <c r="G114" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B115" s="15">
-        <v>1</v>
-      </c>
-      <c r="C115" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D115" s="15">
+      <c r="B115" s="14">
+        <v>1</v>
+      </c>
+      <c r="C115" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D115" s="14">
         <v>-83.085526805000001</v>
       </c>
-      <c r="E115" s="15">
+      <c r="E115" s="14">
         <v>149</v>
       </c>
-      <c r="F115" s="15">
-        <v>0</v>
-      </c>
-      <c r="G115" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="15" t="s">
+      <c r="F115" s="14">
+        <v>0</v>
+      </c>
+      <c r="G115" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B116" s="15">
-        <v>1</v>
-      </c>
-      <c r="C116" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D116" s="15">
+      <c r="B116" s="14">
+        <v>1</v>
+      </c>
+      <c r="C116" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D116" s="14">
         <v>-90.091340471999999</v>
       </c>
-      <c r="E116" s="15">
+      <c r="E116" s="14">
         <v>150</v>
       </c>
-      <c r="F116" s="15">
-        <v>0</v>
-      </c>
-      <c r="G116" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="15" t="s">
+      <c r="F116" s="14">
+        <v>0</v>
+      </c>
+      <c r="G116" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B117" s="15">
-        <v>1</v>
-      </c>
-      <c r="C117" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D117" s="15">
+      <c r="B117" s="14">
+        <v>1</v>
+      </c>
+      <c r="C117" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D117" s="14">
         <v>-97.064791365000005</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E117" s="14">
         <v>151</v>
       </c>
-      <c r="F117" s="15">
-        <v>0</v>
-      </c>
-      <c r="G117" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="15" t="s">
+      <c r="F117" s="14">
+        <v>0</v>
+      </c>
+      <c r="G117" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B118" s="15">
-        <v>1</v>
-      </c>
-      <c r="C118" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D118" s="15">
+      <c r="B118" s="14">
+        <v>1</v>
+      </c>
+      <c r="C118" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D118" s="14">
         <v>-125.096091505</v>
       </c>
-      <c r="E118" s="15">
+      <c r="E118" s="14">
         <v>152</v>
       </c>
-      <c r="F118" s="15">
-        <v>0</v>
-      </c>
-      <c r="G118" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="15" t="s">
+      <c r="F118" s="14">
+        <v>0</v>
+      </c>
+      <c r="G118" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="B119" s="15">
-        <v>1</v>
-      </c>
-      <c r="C119" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D119" s="15">
+      <c r="B119" s="14">
+        <v>1</v>
+      </c>
+      <c r="C119" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D119" s="14">
         <v>-111.080441435</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="14">
         <v>153</v>
       </c>
-      <c r="F119" s="15">
-        <v>0</v>
-      </c>
-      <c r="G119" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="15" t="s">
+      <c r="F119" s="14">
+        <v>0</v>
+      </c>
+      <c r="G119" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="B120" s="15">
-        <v>1</v>
-      </c>
-      <c r="C120" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D120" s="15">
+      <c r="B120" s="14">
+        <v>1</v>
+      </c>
+      <c r="C120" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D120" s="14">
         <v>-145.085920765</v>
       </c>
-      <c r="E120" s="15">
+      <c r="E120" s="14">
         <v>154</v>
       </c>
-      <c r="F120" s="15">
-        <v>0</v>
-      </c>
-      <c r="G120" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="15" t="s">
+      <c r="F120" s="14">
+        <v>0</v>
+      </c>
+      <c r="G120" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B121" s="15">
-        <v>1</v>
-      </c>
-      <c r="C121" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D121" s="15">
+      <c r="B121" s="14">
+        <v>1</v>
+      </c>
+      <c r="C121" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D121" s="14">
         <v>-111.116826945</v>
       </c>
-      <c r="E121" s="15">
+      <c r="E121" s="14">
         <v>155</v>
       </c>
-      <c r="F121" s="15">
-        <v>0</v>
-      </c>
-      <c r="G121" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="15" t="s">
+      <c r="F121" s="14">
+        <v>0</v>
+      </c>
+      <c r="G121" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B122" s="15">
-        <v>1</v>
-      </c>
-      <c r="C122" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D122" s="15">
+      <c r="B122" s="14">
+        <v>1</v>
+      </c>
+      <c r="C122" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D122" s="14">
         <v>-96.065519662</v>
       </c>
-      <c r="E122" s="15">
+      <c r="E122" s="14">
         <v>156</v>
       </c>
-      <c r="F122" s="15">
-        <v>0</v>
-      </c>
-      <c r="G122" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="15" t="s">
+      <c r="F122" s="14">
+        <v>0</v>
+      </c>
+      <c r="G122" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B123" s="15">
-        <v>1</v>
-      </c>
-      <c r="C123" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D123" s="15">
+      <c r="B123" s="14">
+        <v>1</v>
+      </c>
+      <c r="C123" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D123" s="14">
         <v>-48.080775772000003</v>
       </c>
-      <c r="E123" s="15">
+      <c r="E123" s="14">
         <v>157</v>
       </c>
-      <c r="F123" s="15">
-        <v>0</v>
-      </c>
-      <c r="G123" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="15" t="s">
+      <c r="F123" s="14">
+        <v>0</v>
+      </c>
+      <c r="G123" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B124" s="15">
-        <v>1</v>
-      </c>
-      <c r="C124" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D124" s="15">
+      <c r="B124" s="14">
+        <v>1</v>
+      </c>
+      <c r="C124" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D124" s="14">
         <v>-150.09134047200001</v>
       </c>
-      <c r="E124" s="15">
+      <c r="E124" s="14">
         <v>158</v>
       </c>
-      <c r="F124" s="15">
-        <v>0</v>
-      </c>
-      <c r="G124" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="15" t="s">
+      <c r="F124" s="14">
+        <v>0</v>
+      </c>
+      <c r="G124" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B125" s="15">
-        <v>1</v>
-      </c>
-      <c r="C125" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D125" s="15">
+      <c r="B125" s="14">
+        <v>1</v>
+      </c>
+      <c r="C125" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D125" s="14">
         <v>-100.07569040200001</v>
       </c>
-      <c r="E125" s="15">
+      <c r="E125" s="14">
         <v>159</v>
       </c>
-      <c r="F125" s="15">
-        <v>0</v>
-      </c>
-      <c r="G125" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="15" t="s">
+      <c r="F125" s="14">
+        <v>0</v>
+      </c>
+      <c r="G125" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B126" s="15">
-        <v>1</v>
-      </c>
-      <c r="C126" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D126" s="15">
+      <c r="B126" s="14">
+        <v>1</v>
+      </c>
+      <c r="C126" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D126" s="14">
         <v>-60.080775772000003</v>
       </c>
-      <c r="E126" s="15">
+      <c r="E126" s="14">
         <v>160</v>
       </c>
-      <c r="F126" s="15">
-        <v>0</v>
-      </c>
-      <c r="G126" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="15" t="s">
+      <c r="F126" s="14">
+        <v>0</v>
+      </c>
+      <c r="G126" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B127" s="15">
-        <v>1</v>
-      </c>
-      <c r="C127" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D127" s="15">
+      <c r="B127" s="14">
+        <v>1</v>
+      </c>
+      <c r="C127" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D127" s="14">
         <v>-120.101905172</v>
       </c>
-      <c r="E127" s="15">
+      <c r="E127" s="14">
         <v>161</v>
       </c>
-      <c r="F127" s="15">
-        <v>0</v>
-      </c>
-      <c r="G127" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="15" t="s">
+      <c r="F127" s="14">
+        <v>0</v>
+      </c>
+      <c r="G127" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="B128" s="15">
-        <v>1</v>
-      </c>
-      <c r="C128" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D128" s="15">
+      <c r="B128" s="14">
+        <v>1</v>
+      </c>
+      <c r="C128" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D128" s="14">
         <v>-177.0394</v>
       </c>
-      <c r="E128" s="15">
+      <c r="E128" s="14">
         <v>162</v>
       </c>
-      <c r="F128" s="15">
-        <v>0</v>
-      </c>
-      <c r="G128" s="15">
+      <c r="F128" s="14">
+        <v>0</v>
+      </c>
+      <c r="G128" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="15" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B129" s="15">
-        <v>1</v>
-      </c>
-      <c r="C129" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D129" s="15">
+      <c r="B129" s="14">
+        <v>1</v>
+      </c>
+      <c r="C129" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D129" s="14">
         <v>-195.04995291</v>
       </c>
-      <c r="E129" s="15">
+      <c r="E129" s="14">
         <v>163</v>
       </c>
-      <c r="F129" s="15">
-        <v>0</v>
-      </c>
-      <c r="G129" s="15">
+      <c r="F129" s="14">
+        <v>0</v>
+      </c>
+      <c r="G129" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="15" t="s">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="B130" s="15">
-        <v>1</v>
-      </c>
-      <c r="C130" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D130" s="15">
+      <c r="B130" s="14">
+        <v>1</v>
+      </c>
+      <c r="C130" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D130" s="14">
         <v>-213.06045291000001</v>
       </c>
-      <c r="E130" s="15">
+      <c r="E130" s="14">
         <v>164</v>
       </c>
-      <c r="F130" s="15">
-        <v>0</v>
-      </c>
-      <c r="G130" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="15" t="s">
+      <c r="F130" s="14">
+        <v>0</v>
+      </c>
+      <c r="G130" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="B131" s="15">
-        <v>1</v>
-      </c>
-      <c r="C131" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D131" s="15">
+      <c r="B131" s="14">
+        <v>1</v>
+      </c>
+      <c r="C131" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D131" s="14">
         <v>-231.07105290999999</v>
       </c>
-      <c r="E131" s="15">
+      <c r="E131" s="14">
         <v>165</v>
       </c>
-      <c r="F131" s="15">
-        <v>0</v>
-      </c>
-      <c r="G131" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A132" s="15" t="s">
+      <c r="F131" s="14">
+        <v>0</v>
+      </c>
+      <c r="G131" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="B132" s="15">
-        <v>1</v>
-      </c>
-      <c r="C132" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D132" s="15">
+      <c r="B132" s="14">
+        <v>1</v>
+      </c>
+      <c r="C132" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D132" s="14">
         <v>-259.06595291000002</v>
       </c>
-      <c r="E132" s="15">
+      <c r="E132" s="14">
         <v>166</v>
       </c>
-      <c r="F132" s="15">
-        <v>0</v>
-      </c>
-      <c r="G132" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A133" s="15" t="s">
+      <c r="F132" s="14">
+        <v>0</v>
+      </c>
+      <c r="G132" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B133" s="15">
-        <v>1</v>
-      </c>
-      <c r="C133" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D133" s="15">
+      <c r="B133" s="14">
+        <v>1</v>
+      </c>
+      <c r="C133" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D133" s="14">
         <v>-55.038972909999998</v>
       </c>
-      <c r="E133" s="15">
+      <c r="E133" s="14">
         <v>167</v>
       </c>
-      <c r="F133" s="15">
-        <v>0</v>
-      </c>
-      <c r="G133" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
+      <c r="F133" s="14">
+        <v>0</v>
+      </c>
+      <c r="G133" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="B134" s="15">
-        <v>1</v>
-      </c>
-      <c r="C134" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D134" s="15">
+      <c r="B134" s="14">
+        <v>1</v>
+      </c>
+      <c r="C134" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D134" s="14">
         <v>-83.033882910000003</v>
       </c>
-      <c r="E134" s="15">
+      <c r="E134" s="14">
         <v>168</v>
       </c>
-      <c r="F134" s="15">
-        <v>0</v>
-      </c>
-      <c r="G134" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A135" s="15" t="s">
+      <c r="F134" s="14">
+        <v>0</v>
+      </c>
+      <c r="G134" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="B135" s="15">
-        <v>1</v>
-      </c>
-      <c r="C135" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D135" s="15">
+      <c r="B135" s="14">
+        <v>1</v>
+      </c>
+      <c r="C135" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D135" s="14">
         <v>-132.10195290999999</v>
       </c>
-      <c r="E135" s="15">
+      <c r="E135" s="14">
         <v>169</v>
       </c>
-      <c r="F135" s="15">
-        <v>0</v>
-      </c>
-      <c r="G135" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="15" t="s">
+      <c r="F135" s="14">
+        <v>0</v>
+      </c>
+      <c r="G135" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="B136" s="15">
-        <v>1</v>
-      </c>
-      <c r="C136" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D136" s="15">
+      <c r="B136" s="14">
+        <v>1</v>
+      </c>
+      <c r="C136" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D136" s="14">
         <v>-118.08625291</v>
       </c>
-      <c r="E136" s="15">
+      <c r="E136" s="14">
         <v>170</v>
       </c>
-      <c r="F136" s="15">
-        <v>0</v>
-      </c>
-      <c r="G136" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="15" t="s">
+      <c r="F136" s="14">
+        <v>0</v>
+      </c>
+      <c r="G136" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B137" s="15">
-        <v>1</v>
-      </c>
-      <c r="C137" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D137" s="15">
+      <c r="B137" s="14">
+        <v>1</v>
+      </c>
+      <c r="C137" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D137" s="14">
         <v>-48.002822909999999</v>
       </c>
-      <c r="E137" s="15">
+      <c r="E137" s="14">
         <v>171</v>
       </c>
-      <c r="F137" s="15">
-        <v>0</v>
-      </c>
-      <c r="G137" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
+      <c r="F137" s="14">
+        <v>0</v>
+      </c>
+      <c r="G137" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="B138" s="15">
-        <v>1</v>
-      </c>
-      <c r="C138" s="15">
-        <v>-1</v>
-      </c>
-      <c r="D138" s="15">
+      <c r="B138" s="14">
+        <v>1</v>
+      </c>
+      <c r="C138" s="14">
+        <v>-1</v>
+      </c>
+      <c r="D138" s="14">
         <v>-119.04915291</v>
       </c>
-      <c r="E138" s="15">
+      <c r="E138" s="14">
         <v>172</v>
       </c>
-      <c r="F138" s="15">
-        <v>0</v>
-      </c>
-      <c r="G138" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="15" t="s">
+      <c r="F138" s="14">
+        <v>0</v>
+      </c>
+      <c r="G138" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B139" s="15">
-        <v>1</v>
-      </c>
-      <c r="C139" s="15">
+      <c r="B139" s="14">
+        <v>1</v>
+      </c>
+      <c r="C139" s="14">
         <v>-1</v>
       </c>
       <c r="D139">
         <f>-(162.05283-D2)</f>
         <v>-163.06010645500001</v>
       </c>
-      <c r="E139" s="15">
+      <c r="E139" s="14">
         <v>173</v>
       </c>
-      <c r="F139" s="15">
-        <v>0</v>
-      </c>
-      <c r="G139" s="15">
+      <c r="F139" s="14">
+        <v>0</v>
+      </c>
+      <c r="G139" s="14">
         <v>0.75</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A140" s="15" t="s">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B140" s="15">
-        <v>1</v>
-      </c>
-      <c r="C140" s="15">
+      <c r="B140" s="14">
+        <v>1</v>
+      </c>
+      <c r="C140" s="14">
         <v>1</v>
       </c>
       <c r="D140">
         <f>D139+D79+1.0073</f>
         <v>-179.09138213500003</v>
       </c>
-      <c r="E140" s="15">
+      <c r="E140" s="14">
         <v>174</v>
       </c>
-      <c r="F140" s="15">
-        <v>0</v>
-      </c>
-      <c r="G140" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="15" t="s">
+      <c r="F140" s="14">
+        <v>0</v>
+      </c>
+      <c r="G140" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="B141" s="15">
-        <v>1</v>
-      </c>
-      <c r="C141" s="15">
+      <c r="B141" s="14">
+        <v>1</v>
+      </c>
+      <c r="C141" s="14">
         <v>1</v>
       </c>
       <c r="D141">
         <f>D139+D82+1.0073</f>
         <v>-195.08629676500001</v>
       </c>
-      <c r="E141" s="15">
+      <c r="E141" s="14">
         <v>175</v>
       </c>
-      <c r="F141" s="15">
-        <v>0</v>
-      </c>
-      <c r="G141" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="15" t="s">
+      <c r="F141" s="14">
+        <v>0</v>
+      </c>
+      <c r="G141" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="B142" s="15">
-        <v>1</v>
-      </c>
-      <c r="C142" s="15">
+      <c r="B142" s="14">
+        <v>1</v>
+      </c>
+      <c r="C142" s="14">
         <v>1</v>
       </c>
       <c r="D142">
         <f>D139+D69+1.0073</f>
         <v>-207.08629676500001</v>
       </c>
-      <c r="E142" s="15">
+      <c r="E142" s="14">
         <v>176</v>
       </c>
-      <c r="F142" s="15">
-        <v>0</v>
-      </c>
-      <c r="G142" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="15" t="s">
+      <c r="F142" s="14">
+        <v>0</v>
+      </c>
+      <c r="G142" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="B143" s="15">
-        <v>1</v>
-      </c>
-      <c r="C143" s="15">
+      <c r="B143" s="14">
+        <v>1</v>
+      </c>
+      <c r="C143" s="14">
         <v>1</v>
       </c>
       <c r="D143">
         <f>D139+D98+1.0073</f>
         <v>-223.08121231000001</v>
       </c>
-      <c r="E143" s="15">
+      <c r="E143" s="14">
         <v>177</v>
       </c>
-      <c r="F143" s="15">
-        <v>0</v>
-      </c>
-      <c r="G143" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="15" t="s">
+      <c r="F143" s="14">
+        <v>0</v>
+      </c>
+      <c r="G143" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="B144" s="15">
-        <v>1</v>
-      </c>
-      <c r="C144" s="15">
+      <c r="B144" s="14">
+        <v>1</v>
+      </c>
+      <c r="C144" s="14">
         <v>1</v>
       </c>
       <c r="D144">
         <f>-(2*162.05283-D2)</f>
         <v>-325.11293645500001</v>
       </c>
-      <c r="E144" s="15">
+      <c r="E144" s="14">
         <v>178</v>
       </c>
-      <c r="F144" s="15">
-        <v>0</v>
-      </c>
-      <c r="G144" s="15">
+      <c r="F144" s="14">
+        <v>0</v>
+      </c>
+      <c r="G144" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B145" s="14">
+        <v>1</v>
+      </c>
+      <c r="C145" s="14">
+        <v>1</v>
+      </c>
+      <c r="D145">
+        <f>-(60.02113-D2)</f>
+        <v>-61.028406455000002</v>
+      </c>
+      <c r="E145" s="14">
+        <v>179</v>
+      </c>
+      <c r="F145" s="14">
+        <v>0</v>
+      </c>
+      <c r="G145" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="B146" s="14">
+        <v>1</v>
+      </c>
+      <c r="C146" s="14">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <f>-(15.02348-D2)</f>
+        <v>-16.030756454999999</v>
+      </c>
+      <c r="E146" s="14">
+        <v>180</v>
+      </c>
+      <c r="F146" s="14">
+        <v>0</v>
+      </c>
+      <c r="G146" s="14">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>